<commit_message>
added a inhalation model and ongoing struggles to resolve mass balance issue
</commit_message>
<xml_diff>
--- a/Parameter supplementary data .xlsx
+++ b/Parameter supplementary data .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joris\Documents\PBK\Cinnamaldehyde-pbk\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Joris\Toxicology and Environmental Health\Master stage\R\Cinnamaldehyde PBK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55422CA2-4603-403B-A0A2-B495DF55696F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02BD2F8-D0D0-4DB3-BB57-8B132A272E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31EFE8C3-DD10-4F56-8B9A-3502E68B8CEB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="265">
   <si>
     <t xml:space="preserve">Parameter </t>
   </si>
@@ -897,12 +897,63 @@
   <si>
     <t>This is the remaning slowly perfused tissue after subtracting other slowly perfused compartments</t>
   </si>
+  <si>
+    <t>104-55-2</t>
+  </si>
+  <si>
+    <t>3-phenyl-2-propenal</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Sa</t>
+  </si>
+  <si>
+    <t>CAS-number</t>
+  </si>
+  <si>
+    <t>Compound name</t>
+  </si>
+  <si>
+    <t>Faeces</t>
+  </si>
+  <si>
+    <t>Urine</t>
+  </si>
+  <si>
+    <t>Breath</t>
+  </si>
+  <si>
+    <t>Skin</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Saliva</t>
+  </si>
+  <si>
+    <t>Henry' constant @ 310.15 K [conc_water/conc_air]</t>
+  </si>
+  <si>
+    <t>Blood:Air partition coefficient [conc_blood/conc_air]</t>
+  </si>
+  <si>
+    <t>Fat:Air partition coefficient  [conc_fat/conc_air]</t>
+  </si>
+  <si>
+    <t>Fat_Blood partition coefficient  [conc_fat/conc_blood]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -946,6 +997,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -960,7 +1025,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -968,12 +1033,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1010,10 +1136,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Ongeldig" xfId="1" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard 2" xfId="2" xr:uid="{DE7BC18A-9D54-48A0-AB30-07C48903A88E}"/>
+    <cellStyle name="Standard 2" xfId="3" xr:uid="{8BE6A642-AF34-43F4-A01E-4F8E076EA935}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1325,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D684224-74AE-4DFE-B7FF-DE9B6310C4D9}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K87" sqref="K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2356,6 +2509,79 @@
       </c>
       <c r="D66" s="5" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="86" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A86" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="C86" s="23" t="s">
+        <v>254</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E86" s="23" t="s">
+        <v>256</v>
+      </c>
+      <c r="F86" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="G86" s="23" t="s">
+        <v>258</v>
+      </c>
+      <c r="H86" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="I86" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="J86" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="K86" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="L86" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="M86" s="26" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B87" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="D87" s="18"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="J87" s="20">
+        <v>873.10334785411487</v>
+      </c>
+      <c r="K87" s="20">
+        <v>274.83920626249699</v>
+      </c>
+      <c r="L87" s="20">
+        <v>80886.100486578129</v>
+      </c>
+      <c r="M87" s="19">
+        <v>294.30335499268068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>